<commit_message>
Implemented alternative thermo_processor using ViennaRNA due to easier installation
</commit_message>
<xml_diff>
--- a/ddprimer/tests/Primers/Primers_fasta1.xlsx
+++ b/ddprimer/tests/Primers/Primers_fasta1.xlsx
@@ -683,7 +683,7 @@
         <v>1.418635688603434</v>
       </c>
       <c r="E3" s="6" t="n">
-        <v>0</v>
+        <v>-0.4000000059604645</v>
       </c>
       <c r="F3" s="6" t="n">
         <v>0.007</v>
@@ -726,7 +726,7 @@
         <v>6.534246572323525</v>
       </c>
       <c r="R3" s="6" t="n">
-        <v>-0.8420321941375732</v>
+        <v>-1.600000023841858</v>
       </c>
       <c r="S3" s="6" t="n">
         <v>1.51e-06</v>
@@ -746,7 +746,7 @@
         <v>52.63157894736842</v>
       </c>
       <c r="X3" s="6" t="n">
-        <v>-8.800433158874512</v>
+        <v>-30.5</v>
       </c>
       <c r="Y3" s="6" t="inlineStr">
         <is>
@@ -777,7 +777,7 @@
         <v>1.684335183667191</v>
       </c>
       <c r="E4" s="6" t="n">
-        <v>-0.8030736446380615</v>
+        <v>-1.5</v>
       </c>
       <c r="F4" s="6" t="n">
         <v>0.007</v>
@@ -797,7 +797,7 @@
         <v>2.218872212289785</v>
       </c>
       <c r="K4" s="6" t="n">
-        <v>0</v>
+        <v>-0.699999988079071</v>
       </c>
       <c r="L4" s="6" t="n">
         <v>0.007</v>
@@ -820,7 +820,7 @@
         <v>6.534246572323525</v>
       </c>
       <c r="R4" s="6" t="n">
-        <v>-0.8420321941375732</v>
+        <v>-1.600000023841858</v>
       </c>
       <c r="S4" s="6" t="n">
         <v>1.51e-06</v>
@@ -840,7 +840,7 @@
         <v>52.63157894736842</v>
       </c>
       <c r="X4" s="6" t="n">
-        <v>-8.800433158874512</v>
+        <v>-18.60000038146973</v>
       </c>
       <c r="Y4" s="6" t="inlineStr">
         <is>
@@ -871,7 +871,7 @@
         <v>1.385652307599617</v>
       </c>
       <c r="E5" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F5" s="6" t="n">
         <v>0.007</v>
@@ -889,7 +889,7 @@
         <v>1.164318971265448</v>
       </c>
       <c r="K5" s="6" t="n">
-        <v>0</v>
+        <v>-0.300000011920929</v>
       </c>
       <c r="L5" s="6" t="n">
         <v>0.007</v>
@@ -912,7 +912,7 @@
         <v>6.698646749007992</v>
       </c>
       <c r="R5" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>-2</v>
       </c>
       <c r="S5" s="6" t="n">
         <v>1.51e-06</v>
@@ -932,7 +932,7 @@
         <v>51.9607843137255</v>
       </c>
       <c r="X5" s="6" t="n">
-        <v>-5.947404861450195</v>
+        <v>-25.10000038146973</v>
       </c>
       <c r="Y5" s="6" t="inlineStr">
         <is>
@@ -963,7 +963,7 @@
         <v>1.681626298122911</v>
       </c>
       <c r="E6" s="6" t="n">
-        <v>-0.8097348213195801</v>
+        <v>0</v>
       </c>
       <c r="F6" s="6" t="n">
         <v>0.007</v>
@@ -983,7 +983,7 @@
         <v>1.816617440952985</v>
       </c>
       <c r="K6" s="6" t="n">
-        <v>0</v>
+        <v>-3.900000095367432</v>
       </c>
       <c r="L6" s="6" t="n">
         <v>0.007</v>
@@ -1006,7 +1006,7 @@
         <v>7.795123969468762</v>
       </c>
       <c r="R6" s="6" t="n">
-        <v>-1.419864654541016</v>
+        <v>-2</v>
       </c>
       <c r="S6" s="6" t="n">
         <v>5.4e-07</v>
@@ -1026,7 +1026,7 @@
         <v>51.45631067961165</v>
       </c>
       <c r="X6" s="6" t="n">
-        <v>-5.947404861450195</v>
+        <v>-24.10000038146973</v>
       </c>
       <c r="Y6" s="6" t="inlineStr">
         <is>
@@ -1077,7 +1077,7 @@
         <v>1.07008396900078</v>
       </c>
       <c r="K7" s="6" t="n">
-        <v>0</v>
+        <v>-1.700000047683716</v>
       </c>
       <c r="L7" s="6" t="n">
         <v>0.007</v>
@@ -1100,7 +1100,7 @@
         <v>6.278414617755686</v>
       </c>
       <c r="R7" s="6" t="n">
-        <v>0</v>
+        <v>-4.300000190734863</v>
       </c>
       <c r="S7" s="6" t="n">
         <v>1.51e-06</v>
@@ -1120,7 +1120,7 @@
         <v>55.44554455445545</v>
       </c>
       <c r="X7" s="6" t="n">
-        <v>-4.261404037475586</v>
+        <v>-26.29999923706055</v>
       </c>
       <c r="Y7" s="6" t="inlineStr">
         <is>
@@ -1151,7 +1151,7 @@
         <v>1.457016311382517</v>
       </c>
       <c r="E8" s="6" t="n">
-        <v>-0.7797346115112305</v>
+        <v>-0.300000011920929</v>
       </c>
       <c r="F8" s="6" t="n">
         <v>0.002</v>
@@ -1171,7 +1171,7 @@
         <v>1.708555007319251</v>
       </c>
       <c r="K8" s="6" t="n">
-        <v>0</v>
+        <v>-0.4000000059604645</v>
       </c>
       <c r="L8" s="6" t="n">
         <v>0.007</v>
@@ -1214,7 +1214,7 @@
         <v>53.44827586206896</v>
       </c>
       <c r="X8" s="6" t="n">
-        <v>-5.429211139678955</v>
+        <v>-23.39999961853027</v>
       </c>
       <c r="Y8" s="6" t="inlineStr">
         <is>
@@ -1245,7 +1245,7 @@
         <v>1.865360794074377</v>
       </c>
       <c r="E9" s="6" t="n">
-        <v>0</v>
+        <v>-2.400000095367432</v>
       </c>
       <c r="F9" s="6" t="n">
         <v>0.002</v>
@@ -1265,7 +1265,7 @@
         <v>1.919346081889103</v>
       </c>
       <c r="K9" s="6" t="n">
-        <v>0</v>
+        <v>-0.1000000014901161</v>
       </c>
       <c r="L9" s="6" t="n">
         <v>0.002</v>
@@ -1288,7 +1288,7 @@
         <v>7.185476069159051</v>
       </c>
       <c r="R9" s="6" t="n">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="S9" s="6" t="n">
         <v>5.4e-07</v>
@@ -1308,7 +1308,7 @@
         <v>52.29357798165137</v>
       </c>
       <c r="X9" s="6" t="n">
-        <v>-3.461651563644409</v>
+        <v>-30.70000076293945</v>
       </c>
       <c r="Y9" s="6" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
         <v>2.154473936120439</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>0</v>
+        <v>-2.599999904632568</v>
       </c>
       <c r="F10" s="6" t="n">
         <v>0.002</v>
@@ -1382,7 +1382,7 @@
         <v>7.185476069159051</v>
       </c>
       <c r="R10" s="6" t="n">
-        <v>0</v>
+        <v>-2.5</v>
       </c>
       <c r="S10" s="6" t="n">
         <v>5.4e-07</v>
@@ -1402,7 +1402,7 @@
         <v>50</v>
       </c>
       <c r="X10" s="6" t="n">
-        <v>-3.461651563644409</v>
+        <v>-26.39999961853027</v>
       </c>
       <c r="Y10" s="6" t="inlineStr">
         <is>
@@ -1433,7 +1433,7 @@
         <v>1.1220987618692</v>
       </c>
       <c r="E11" s="6" t="n">
-        <v>-0.3097348213195801</v>
+        <v>-0.1000000014901161</v>
       </c>
       <c r="F11" s="6" t="n">
         <v>0.007</v>
@@ -1453,7 +1453,7 @@
         <v>1.396612197889898</v>
       </c>
       <c r="K11" s="6" t="n">
-        <v>0</v>
+        <v>-1.299999952316284</v>
       </c>
       <c r="L11" s="6" t="n">
         <v>0.007</v>
@@ -1476,7 +1476,7 @@
         <v>6.774014645800662</v>
       </c>
       <c r="R11" s="6" t="n">
-        <v>-0.7341697216033936</v>
+        <v>-3.099999904632568</v>
       </c>
       <c r="S11" s="6" t="n">
         <v>1.51e-06</v>
@@ -1496,7 +1496,7 @@
         <v>53.98230088495575</v>
       </c>
       <c r="X11" s="6" t="n">
-        <v>-6.521465301513672</v>
+        <v>-26.60000038146973</v>
       </c>
       <c r="Y11" s="6" t="inlineStr">
         <is>
@@ -1527,7 +1527,7 @@
         <v>1.363968696357801</v>
       </c>
       <c r="E12" s="6" t="n">
-        <v>0</v>
+        <v>-0.699999988079071</v>
       </c>
       <c r="F12" s="6" t="n">
         <v>0.002</v>
@@ -1570,7 +1570,7 @@
         <v>6.774014645800662</v>
       </c>
       <c r="R12" s="6" t="n">
-        <v>-0.7341697216033936</v>
+        <v>-3.099999904632568</v>
       </c>
       <c r="S12" s="6" t="n">
         <v>1.51e-06</v>
@@ -1590,7 +1590,7 @@
         <v>53.96825396825397</v>
       </c>
       <c r="X12" s="6" t="n">
-        <v>-6.521465301513672</v>
+        <v>-30</v>
       </c>
       <c r="Y12" s="6" t="inlineStr">
         <is>
@@ -1684,7 +1684,7 @@
         <v>53.03030303030303</v>
       </c>
       <c r="X13" s="6" t="n">
-        <v>-17.26604652404785</v>
+        <v>-59.90000152587891</v>
       </c>
       <c r="Y13" s="6" t="inlineStr">
         <is>
@@ -1715,7 +1715,7 @@
         <v>1.698923989928222</v>
       </c>
       <c r="E14" s="6" t="n">
-        <v>0</v>
+        <v>-3.299999952316284</v>
       </c>
       <c r="F14" s="6" t="n">
         <v>0.007</v>
@@ -1735,7 +1735,7 @@
         <v>2.677661703245565</v>
       </c>
       <c r="K14" s="6" t="n">
-        <v>-0.790266752243042</v>
+        <v>-0.2000000029802322</v>
       </c>
       <c r="L14" s="6" t="n">
         <v>0.007</v>
@@ -1758,7 +1758,7 @@
         <v>2.295051095305325</v>
       </c>
       <c r="R14" s="6" t="n">
-        <v>-0.9579751491546631</v>
+        <v>-4</v>
       </c>
       <c r="S14" s="6" t="n">
         <v>0.000168</v>
@@ -1776,7 +1776,7 @@
         <v>51.9607843137255</v>
       </c>
       <c r="X14" s="6" t="n">
-        <v>-6.424409866333008</v>
+        <v>-29</v>
       </c>
       <c r="Y14" s="6" t="inlineStr">
         <is>
@@ -1850,7 +1850,7 @@
         <v>0.3401371934283475</v>
       </c>
       <c r="R15" s="6" t="n">
-        <v>-1.617270469665527</v>
+        <v>-4.699999809265137</v>
       </c>
       <c r="S15" s="6" t="n">
         <v>0.002</v>
@@ -1870,7 +1870,7 @@
         <v>52.46913580246913</v>
       </c>
       <c r="X15" s="6" t="n">
-        <v>-10.59030723571777</v>
+        <v>-39.70000076293945</v>
       </c>
       <c r="Y15" s="6" t="inlineStr">
         <is>

</xml_diff>